<commit_message>
Minor updates to quiz spreadsheet and removed migrations from .gitignore
</commit_message>
<xml_diff>
--- a/demo_quiz/Synaptic Demo Quiz.xlsx
+++ b/demo_quiz/Synaptic Demo Quiz.xlsx
@@ -300,10 +300,6 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -348,6 +344,10 @@
     <xf numFmtId="1" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="12" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -448,7 +448,7 @@
         <xdr:cNvPr id="2" name="CustomShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -488,7 +488,7 @@
         <xdr:cNvPr id="3" name="CustomShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -802,7 +802,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -813,21 +813,21 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AC971"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="I13" sqref="I13"/>
+      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="12.42578125"/>
-    <col min="2" max="2" width="59.28515625" style="25" customWidth="1"/>
-    <col min="3" max="6" width="31.85546875" style="21"/>
-    <col min="7" max="7" width="26.28515625"/>
-    <col min="8" max="8" width="28.42578125" customWidth="1"/>
-    <col min="9" max="9" width="28.42578125" style="21" customWidth="1"/>
-    <col min="10" max="10" width="33.140625" style="30"/>
+    <col min="1" max="1" width="6.42578125" customWidth="1"/>
+    <col min="2" max="2" width="59.28515625" style="23" customWidth="1"/>
+    <col min="3" max="6" width="31.85546875" style="19"/>
+    <col min="7" max="7" width="18.85546875" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" customWidth="1"/>
+    <col min="9" max="9" width="28.42578125" style="19" customWidth="1"/>
+    <col min="10" max="10" width="19.7109375" style="28" customWidth="1"/>
     <col min="11" max="12" width="11.42578125"/>
     <col min="14" max="29" width="11.42578125"/>
     <col min="30" max="1027" width="14.42578125"/>
@@ -835,15 +835,15 @@
   <sheetData>
     <row r="1" spans="1:29" ht="18.75" customHeight="1">
       <c r="A1" s="1"/>
-      <c r="B1" s="22"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="31"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="29"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
@@ -866,17 +866,17 @@
     </row>
     <row r="2" spans="1:29" ht="22.5" customHeight="1">
       <c r="A2" s="2"/>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="32"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="30"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
@@ -899,17 +899,17 @@
     </row>
     <row r="3" spans="1:29" ht="29.25" customHeight="1">
       <c r="A3" s="3"/>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
@@ -932,17 +932,17 @@
     </row>
     <row r="4" spans="1:29" ht="15.75" customHeight="1">
       <c r="A4" s="2"/>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="35"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -965,17 +965,17 @@
     </row>
     <row r="5" spans="1:29" ht="15.75" customHeight="1">
       <c r="A5" s="2"/>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
       <c r="G5" s="5"/>
       <c r="H5" s="10"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="33"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="31"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
@@ -998,17 +998,17 @@
     </row>
     <row r="6" spans="1:29" ht="18.75" customHeight="1">
       <c r="A6" s="2"/>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="35"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
@@ -1031,15 +1031,15 @@
     </row>
     <row r="7" spans="1:29" ht="18.75" customHeight="1">
       <c r="A7" s="6"/>
-      <c r="B7" s="24"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="19"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="17"/>
       <c r="G7" s="4"/>
       <c r="H7" s="7"/>
-      <c r="I7" s="26"/>
-      <c r="J7" s="34"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="32"/>
       <c r="K7" s="8"/>
       <c r="L7" s="8"/>
       <c r="M7" s="8"/>
@@ -1062,19 +1062,19 @@
     </row>
     <row r="8" spans="1:29" ht="30">
       <c r="A8" s="7"/>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="20" t="s">
+      <c r="E8" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="20" t="s">
+      <c r="F8" s="18" t="s">
         <v>6</v>
       </c>
       <c r="G8" s="9" t="s">
@@ -1083,10 +1083,10 @@
       <c r="H8" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I8" s="20" t="s">
+      <c r="I8" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="J8" s="35" t="s">
+      <c r="J8" s="33" t="s">
         <v>9</v>
       </c>
       <c r="K8" s="1"/>
@@ -1113,31 +1113,31 @@
       <c r="A9" s="7">
         <v>1</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="F9" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="G9" s="29">
+      <c r="G9" s="27">
         <v>30</v>
       </c>
-      <c r="H9" s="29">
+      <c r="H9" s="27">
         <v>4</v>
       </c>
-      <c r="I9" s="13" t="s">
+      <c r="I9" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="J9" s="29">
+      <c r="J9" s="27">
         <v>2</v>
       </c>
       <c r="K9" s="1"/>
@@ -1164,31 +1164,31 @@
       <c r="A10" s="7">
         <v>2</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E10" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="F10" s="13" t="s">
+      <c r="F10" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="G10" s="29">
+      <c r="G10" s="27">
         <v>20</v>
       </c>
-      <c r="H10" s="29">
+      <c r="H10" s="27">
         <v>3</v>
       </c>
-      <c r="I10" s="27" t="s">
+      <c r="I10" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="J10" s="29"/>
+      <c r="J10" s="27"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
@@ -1213,31 +1213,31 @@
       <c r="A11" s="7">
         <v>3</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="E11" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="F11" s="13" t="s">
+      <c r="F11" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G11" s="29">
+      <c r="G11" s="27">
         <v>20</v>
       </c>
-      <c r="H11" s="29">
+      <c r="H11" s="27">
         <v>1</v>
       </c>
-      <c r="I11" s="13" t="s">
+      <c r="I11" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="J11" s="29">
+      <c r="J11" s="27">
         <v>2</v>
       </c>
       <c r="K11" s="1"/>
@@ -1264,29 +1264,29 @@
       <c r="A12" s="7">
         <v>4</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="E12" s="13" t="s">
+      <c r="E12" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="F12" s="13" t="s">
+      <c r="F12" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="G12" s="29">
+      <c r="G12" s="27">
         <v>30</v>
       </c>
-      <c r="H12" s="29">
+      <c r="H12" s="27">
         <v>1</v>
       </c>
-      <c r="I12" s="13"/>
-      <c r="J12" s="29"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="27"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
@@ -1311,29 +1311,29 @@
       <c r="A13" s="7">
         <v>5</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="E13" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="F13" s="13" t="s">
+      <c r="F13" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="G13" s="29">
+      <c r="G13" s="27">
         <v>30</v>
       </c>
-      <c r="H13" s="29">
+      <c r="H13" s="27">
         <v>2</v>
       </c>
-      <c r="I13" s="13"/>
-      <c r="J13" s="29"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="27"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
@@ -1358,15 +1358,15 @@
       <c r="A14" s="7">
         <v>6</v>
       </c>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="29"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="29"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="27"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
@@ -1391,15 +1391,15 @@
       <c r="A15" s="7">
         <v>7</v>
       </c>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="29"/>
-      <c r="H15" s="29"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="29"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="27"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
@@ -1424,15 +1424,15 @@
       <c r="A16" s="7">
         <v>8</v>
       </c>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="29"/>
-      <c r="H16" s="29"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="29"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="27"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
@@ -1457,15 +1457,15 @@
       <c r="A17" s="7">
         <v>9</v>
       </c>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="29"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="29"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="27"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
@@ -1490,15 +1490,15 @@
       <c r="A18" s="7">
         <v>10</v>
       </c>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="29"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="29"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="27"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
@@ -1523,15 +1523,15 @@
       <c r="A19" s="7">
         <v>11</v>
       </c>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="29"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="29"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="27"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
@@ -1556,15 +1556,15 @@
       <c r="A20" s="7">
         <v>12</v>
       </c>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="29"/>
-      <c r="H20" s="29"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="29"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="27"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
@@ -1589,15 +1589,15 @@
       <c r="A21" s="7">
         <v>13</v>
       </c>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="29"/>
-      <c r="H21" s="29"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="29"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="27"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="27"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
@@ -1622,15 +1622,15 @@
       <c r="A22" s="7">
         <v>14</v>
       </c>
-      <c r="B22" s="13"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="29"/>
-      <c r="H22" s="29"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="29"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="27"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="27"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
@@ -1655,15 +1655,15 @@
       <c r="A23" s="7">
         <v>15</v>
       </c>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="29"/>
-      <c r="H23" s="29"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="29"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="27"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="27"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
@@ -1688,15 +1688,15 @@
       <c r="A24" s="7">
         <v>16</v>
       </c>
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="29"/>
-      <c r="H24" s="29"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="29"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="27"/>
+      <c r="H24" s="27"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="27"/>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
@@ -1721,15 +1721,15 @@
       <c r="A25" s="7">
         <v>17</v>
       </c>
-      <c r="B25" s="13"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="29"/>
-      <c r="H25" s="29"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="29"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="27"/>
+      <c r="H25" s="27"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="27"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
@@ -1754,15 +1754,15 @@
       <c r="A26" s="7">
         <v>18</v>
       </c>
-      <c r="B26" s="13"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="29"/>
-      <c r="H26" s="29"/>
-      <c r="I26" s="13"/>
-      <c r="J26" s="29"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="27"/>
+      <c r="H26" s="27"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="27"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
@@ -1787,15 +1787,15 @@
       <c r="A27" s="7">
         <v>19</v>
       </c>
-      <c r="B27" s="13"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="29"/>
-      <c r="H27" s="29"/>
-      <c r="I27" s="13"/>
-      <c r="J27" s="29"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="27"/>
+      <c r="H27" s="27"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="27"/>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
@@ -1820,15 +1820,15 @@
       <c r="A28" s="7">
         <v>20</v>
       </c>
-      <c r="B28" s="13"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="29"/>
-      <c r="H28" s="29"/>
-      <c r="I28" s="13"/>
-      <c r="J28" s="29"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="27"/>
+      <c r="H28" s="27"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="27"/>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
@@ -1853,15 +1853,15 @@
       <c r="A29" s="7">
         <v>21</v>
       </c>
-      <c r="B29" s="13"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="29"/>
-      <c r="H29" s="29"/>
-      <c r="I29" s="13"/>
-      <c r="J29" s="29"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="27"/>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
@@ -1886,15 +1886,15 @@
       <c r="A30" s="7">
         <v>22</v>
       </c>
-      <c r="B30" s="13"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="29"/>
-      <c r="H30" s="29"/>
-      <c r="I30" s="13"/>
-      <c r="J30" s="29"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="27"/>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
@@ -1919,15 +1919,15 @@
       <c r="A31" s="7">
         <v>23</v>
       </c>
-      <c r="B31" s="13"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="29"/>
-      <c r="H31" s="29"/>
-      <c r="I31" s="13"/>
-      <c r="J31" s="29"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="27"/>
+      <c r="H31" s="27"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="27"/>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
@@ -1952,15 +1952,15 @@
       <c r="A32" s="7">
         <v>24</v>
       </c>
-      <c r="B32" s="13"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="29"/>
-      <c r="H32" s="29"/>
-      <c r="I32" s="13"/>
-      <c r="J32" s="29"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="27"/>
+      <c r="H32" s="27"/>
+      <c r="I32" s="11"/>
+      <c r="J32" s="27"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
@@ -1985,15 +1985,15 @@
       <c r="A33" s="7">
         <v>25</v>
       </c>
-      <c r="B33" s="13"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="29"/>
-      <c r="H33" s="29"/>
-      <c r="I33" s="13"/>
-      <c r="J33" s="29"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="27"/>
+      <c r="H33" s="27"/>
+      <c r="I33" s="11"/>
+      <c r="J33" s="27"/>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
@@ -2018,15 +2018,15 @@
       <c r="A34" s="7">
         <v>26</v>
       </c>
-      <c r="B34" s="13"/>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="29"/>
-      <c r="H34" s="29"/>
-      <c r="I34" s="13"/>
-      <c r="J34" s="29"/>
+      <c r="B34" s="11"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="27"/>
+      <c r="H34" s="27"/>
+      <c r="I34" s="11"/>
+      <c r="J34" s="27"/>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
@@ -2051,15 +2051,15 @@
       <c r="A35" s="7">
         <v>27</v>
       </c>
-      <c r="B35" s="13"/>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="29"/>
-      <c r="H35" s="29"/>
-      <c r="I35" s="13"/>
-      <c r="J35" s="29"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="27"/>
+      <c r="H35" s="27"/>
+      <c r="I35" s="11"/>
+      <c r="J35" s="27"/>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
@@ -2084,15 +2084,15 @@
       <c r="A36" s="7">
         <v>28</v>
       </c>
-      <c r="B36" s="13"/>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="29"/>
-      <c r="H36" s="29"/>
-      <c r="I36" s="13"/>
-      <c r="J36" s="29"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="27"/>
+      <c r="H36" s="27"/>
+      <c r="I36" s="11"/>
+      <c r="J36" s="27"/>
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
@@ -2117,15 +2117,15 @@
       <c r="A37" s="7">
         <v>29</v>
       </c>
-      <c r="B37" s="13"/>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="29"/>
-      <c r="H37" s="29"/>
-      <c r="I37" s="13"/>
-      <c r="J37" s="29"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="27"/>
+      <c r="H37" s="27"/>
+      <c r="I37" s="11"/>
+      <c r="J37" s="27"/>
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
@@ -2150,15 +2150,15 @@
       <c r="A38" s="7">
         <v>30</v>
       </c>
-      <c r="B38" s="13"/>
-      <c r="C38" s="13"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="13"/>
-      <c r="G38" s="29"/>
-      <c r="H38" s="29"/>
-      <c r="I38" s="13"/>
-      <c r="J38" s="29"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
+      <c r="G38" s="27"/>
+      <c r="H38" s="27"/>
+      <c r="I38" s="11"/>
+      <c r="J38" s="27"/>
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
@@ -2183,15 +2183,15 @@
       <c r="A39" s="7">
         <v>31</v>
       </c>
-      <c r="B39" s="13"/>
-      <c r="C39" s="13"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="13"/>
-      <c r="F39" s="13"/>
-      <c r="G39" s="29"/>
-      <c r="H39" s="29"/>
-      <c r="I39" s="13"/>
-      <c r="J39" s="29"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="27"/>
+      <c r="H39" s="27"/>
+      <c r="I39" s="11"/>
+      <c r="J39" s="27"/>
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
@@ -2216,15 +2216,15 @@
       <c r="A40" s="7">
         <v>32</v>
       </c>
-      <c r="B40" s="13"/>
-      <c r="C40" s="13"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="13"/>
-      <c r="F40" s="13"/>
-      <c r="G40" s="29"/>
-      <c r="H40" s="29"/>
-      <c r="I40" s="13"/>
-      <c r="J40" s="29"/>
+      <c r="B40" s="11"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="11"/>
+      <c r="F40" s="11"/>
+      <c r="G40" s="27"/>
+      <c r="H40" s="27"/>
+      <c r="I40" s="11"/>
+      <c r="J40" s="27"/>
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
       <c r="M40" s="1"/>
@@ -2249,15 +2249,15 @@
       <c r="A41" s="7">
         <v>33</v>
       </c>
-      <c r="B41" s="13"/>
-      <c r="C41" s="13"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="13"/>
-      <c r="F41" s="13"/>
-      <c r="G41" s="29"/>
-      <c r="H41" s="29"/>
-      <c r="I41" s="13"/>
-      <c r="J41" s="29"/>
+      <c r="B41" s="11"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="27"/>
+      <c r="H41" s="27"/>
+      <c r="I41" s="11"/>
+      <c r="J41" s="27"/>
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
       <c r="M41" s="1"/>
@@ -2282,15 +2282,15 @@
       <c r="A42" s="7">
         <v>34</v>
       </c>
-      <c r="B42" s="13"/>
-      <c r="C42" s="13"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="13"/>
-      <c r="G42" s="29"/>
-      <c r="H42" s="29"/>
-      <c r="I42" s="13"/>
-      <c r="J42" s="29"/>
+      <c r="B42" s="11"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="11"/>
+      <c r="G42" s="27"/>
+      <c r="H42" s="27"/>
+      <c r="I42" s="11"/>
+      <c r="J42" s="27"/>
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
       <c r="M42" s="1"/>
@@ -2315,15 +2315,15 @@
       <c r="A43" s="7">
         <v>35</v>
       </c>
-      <c r="B43" s="13"/>
-      <c r="C43" s="13"/>
-      <c r="D43" s="13"/>
-      <c r="E43" s="13"/>
-      <c r="F43" s="13"/>
-      <c r="G43" s="29"/>
-      <c r="H43" s="29"/>
-      <c r="I43" s="13"/>
-      <c r="J43" s="29"/>
+      <c r="B43" s="11"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="11"/>
+      <c r="E43" s="11"/>
+      <c r="F43" s="11"/>
+      <c r="G43" s="27"/>
+      <c r="H43" s="27"/>
+      <c r="I43" s="11"/>
+      <c r="J43" s="27"/>
       <c r="K43" s="1"/>
       <c r="L43" s="1"/>
       <c r="M43" s="1"/>
@@ -2348,15 +2348,15 @@
       <c r="A44" s="7">
         <v>36</v>
       </c>
-      <c r="B44" s="13"/>
-      <c r="C44" s="13"/>
-      <c r="D44" s="13"/>
-      <c r="E44" s="13"/>
-      <c r="F44" s="13"/>
-      <c r="G44" s="29"/>
-      <c r="H44" s="29"/>
-      <c r="I44" s="13"/>
-      <c r="J44" s="29"/>
+      <c r="B44" s="11"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="11"/>
+      <c r="E44" s="11"/>
+      <c r="F44" s="11"/>
+      <c r="G44" s="27"/>
+      <c r="H44" s="27"/>
+      <c r="I44" s="11"/>
+      <c r="J44" s="27"/>
       <c r="K44" s="1"/>
       <c r="L44" s="1"/>
       <c r="M44" s="1"/>
@@ -2381,15 +2381,15 @@
       <c r="A45" s="7">
         <v>37</v>
       </c>
-      <c r="B45" s="13"/>
-      <c r="C45" s="13"/>
-      <c r="D45" s="13"/>
-      <c r="E45" s="13"/>
-      <c r="F45" s="13"/>
-      <c r="G45" s="29"/>
-      <c r="H45" s="29"/>
-      <c r="I45" s="13"/>
-      <c r="J45" s="29"/>
+      <c r="B45" s="11"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="11"/>
+      <c r="G45" s="27"/>
+      <c r="H45" s="27"/>
+      <c r="I45" s="11"/>
+      <c r="J45" s="27"/>
       <c r="K45" s="1"/>
       <c r="L45" s="1"/>
       <c r="M45" s="1"/>
@@ -2414,15 +2414,15 @@
       <c r="A46" s="7">
         <v>38</v>
       </c>
-      <c r="B46" s="13"/>
-      <c r="C46" s="13"/>
-      <c r="D46" s="13"/>
-      <c r="E46" s="13"/>
-      <c r="F46" s="13"/>
-      <c r="G46" s="29"/>
-      <c r="H46" s="29"/>
-      <c r="I46" s="13"/>
-      <c r="J46" s="29"/>
+      <c r="B46" s="11"/>
+      <c r="C46" s="11"/>
+      <c r="D46" s="11"/>
+      <c r="E46" s="11"/>
+      <c r="F46" s="11"/>
+      <c r="G46" s="27"/>
+      <c r="H46" s="27"/>
+      <c r="I46" s="11"/>
+      <c r="J46" s="27"/>
       <c r="K46" s="1"/>
       <c r="L46" s="1"/>
       <c r="M46" s="1"/>
@@ -2447,15 +2447,15 @@
       <c r="A47" s="7">
         <v>39</v>
       </c>
-      <c r="B47" s="13"/>
-      <c r="C47" s="13"/>
-      <c r="D47" s="13"/>
-      <c r="E47" s="13"/>
-      <c r="F47" s="13"/>
-      <c r="G47" s="29"/>
-      <c r="H47" s="29"/>
-      <c r="I47" s="13"/>
-      <c r="J47" s="29"/>
+      <c r="B47" s="11"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="11"/>
+      <c r="E47" s="11"/>
+      <c r="F47" s="11"/>
+      <c r="G47" s="27"/>
+      <c r="H47" s="27"/>
+      <c r="I47" s="11"/>
+      <c r="J47" s="27"/>
       <c r="K47" s="1"/>
       <c r="L47" s="1"/>
       <c r="M47" s="1"/>
@@ -2480,15 +2480,15 @@
       <c r="A48" s="7">
         <v>40</v>
       </c>
-      <c r="B48" s="13"/>
-      <c r="C48" s="13"/>
-      <c r="D48" s="13"/>
-      <c r="E48" s="13"/>
-      <c r="F48" s="13"/>
-      <c r="G48" s="29"/>
-      <c r="H48" s="29"/>
-      <c r="I48" s="13"/>
-      <c r="J48" s="29"/>
+      <c r="B48" s="11"/>
+      <c r="C48" s="11"/>
+      <c r="D48" s="11"/>
+      <c r="E48" s="11"/>
+      <c r="F48" s="11"/>
+      <c r="G48" s="27"/>
+      <c r="H48" s="27"/>
+      <c r="I48" s="11"/>
+      <c r="J48" s="27"/>
       <c r="K48" s="1"/>
       <c r="L48" s="1"/>
       <c r="M48" s="1"/>
@@ -2513,15 +2513,15 @@
       <c r="A49" s="7">
         <v>41</v>
       </c>
-      <c r="B49" s="13"/>
-      <c r="C49" s="13"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="13"/>
-      <c r="F49" s="13"/>
-      <c r="G49" s="29"/>
-      <c r="H49" s="29"/>
-      <c r="I49" s="13"/>
-      <c r="J49" s="29"/>
+      <c r="B49" s="11"/>
+      <c r="C49" s="11"/>
+      <c r="D49" s="11"/>
+      <c r="E49" s="11"/>
+      <c r="F49" s="11"/>
+      <c r="G49" s="27"/>
+      <c r="H49" s="27"/>
+      <c r="I49" s="11"/>
+      <c r="J49" s="27"/>
       <c r="K49" s="1"/>
       <c r="L49" s="1"/>
       <c r="M49" s="1"/>
@@ -2546,15 +2546,15 @@
       <c r="A50" s="7">
         <v>42</v>
       </c>
-      <c r="B50" s="13"/>
-      <c r="C50" s="13"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="13"/>
-      <c r="F50" s="13"/>
-      <c r="G50" s="29"/>
-      <c r="H50" s="29"/>
-      <c r="I50" s="13"/>
-      <c r="J50" s="29"/>
+      <c r="B50" s="11"/>
+      <c r="C50" s="11"/>
+      <c r="D50" s="11"/>
+      <c r="E50" s="11"/>
+      <c r="F50" s="11"/>
+      <c r="G50" s="27"/>
+      <c r="H50" s="27"/>
+      <c r="I50" s="11"/>
+      <c r="J50" s="27"/>
       <c r="K50" s="1"/>
       <c r="L50" s="1"/>
       <c r="M50" s="1"/>
@@ -2579,15 +2579,15 @@
       <c r="A51" s="7">
         <v>43</v>
       </c>
-      <c r="B51" s="13"/>
-      <c r="C51" s="13"/>
-      <c r="D51" s="13"/>
-      <c r="E51" s="13"/>
-      <c r="F51" s="13"/>
-      <c r="G51" s="29"/>
-      <c r="H51" s="29"/>
-      <c r="I51" s="13"/>
-      <c r="J51" s="29"/>
+      <c r="B51" s="11"/>
+      <c r="C51" s="11"/>
+      <c r="D51" s="11"/>
+      <c r="E51" s="11"/>
+      <c r="F51" s="11"/>
+      <c r="G51" s="27"/>
+      <c r="H51" s="27"/>
+      <c r="I51" s="11"/>
+      <c r="J51" s="27"/>
       <c r="K51" s="1"/>
       <c r="L51" s="1"/>
       <c r="M51" s="1"/>
@@ -2612,15 +2612,15 @@
       <c r="A52" s="7">
         <v>44</v>
       </c>
-      <c r="B52" s="13"/>
-      <c r="C52" s="13"/>
-      <c r="D52" s="13"/>
-      <c r="E52" s="13"/>
-      <c r="F52" s="13"/>
-      <c r="G52" s="29"/>
-      <c r="H52" s="29"/>
-      <c r="I52" s="13"/>
-      <c r="J52" s="29"/>
+      <c r="B52" s="11"/>
+      <c r="C52" s="11"/>
+      <c r="D52" s="11"/>
+      <c r="E52" s="11"/>
+      <c r="F52" s="11"/>
+      <c r="G52" s="27"/>
+      <c r="H52" s="27"/>
+      <c r="I52" s="11"/>
+      <c r="J52" s="27"/>
       <c r="K52" s="1"/>
       <c r="L52" s="1"/>
       <c r="M52" s="1"/>
@@ -2645,15 +2645,15 @@
       <c r="A53" s="7">
         <v>45</v>
       </c>
-      <c r="B53" s="13"/>
-      <c r="C53" s="13"/>
-      <c r="D53" s="13"/>
-      <c r="E53" s="13"/>
-      <c r="F53" s="13"/>
-      <c r="G53" s="29"/>
-      <c r="H53" s="29"/>
-      <c r="I53" s="13"/>
-      <c r="J53" s="29"/>
+      <c r="B53" s="11"/>
+      <c r="C53" s="11"/>
+      <c r="D53" s="11"/>
+      <c r="E53" s="11"/>
+      <c r="F53" s="11"/>
+      <c r="G53" s="27"/>
+      <c r="H53" s="27"/>
+      <c r="I53" s="11"/>
+      <c r="J53" s="27"/>
       <c r="K53" s="1"/>
       <c r="L53" s="1"/>
       <c r="M53" s="1"/>
@@ -2678,15 +2678,15 @@
       <c r="A54" s="7">
         <v>46</v>
       </c>
-      <c r="B54" s="13"/>
-      <c r="C54" s="13"/>
-      <c r="D54" s="13"/>
-      <c r="E54" s="13"/>
-      <c r="F54" s="13"/>
-      <c r="G54" s="29"/>
-      <c r="H54" s="29"/>
-      <c r="I54" s="13"/>
-      <c r="J54" s="29"/>
+      <c r="B54" s="11"/>
+      <c r="C54" s="11"/>
+      <c r="D54" s="11"/>
+      <c r="E54" s="11"/>
+      <c r="F54" s="11"/>
+      <c r="G54" s="27"/>
+      <c r="H54" s="27"/>
+      <c r="I54" s="11"/>
+      <c r="J54" s="27"/>
       <c r="K54" s="1"/>
       <c r="L54" s="1"/>
       <c r="M54" s="1"/>
@@ -2711,15 +2711,15 @@
       <c r="A55" s="7">
         <v>47</v>
       </c>
-      <c r="B55" s="13"/>
-      <c r="C55" s="13"/>
-      <c r="D55" s="13"/>
-      <c r="E55" s="13"/>
-      <c r="F55" s="13"/>
-      <c r="G55" s="29"/>
-      <c r="H55" s="29"/>
-      <c r="I55" s="13"/>
-      <c r="J55" s="29"/>
+      <c r="B55" s="11"/>
+      <c r="C55" s="11"/>
+      <c r="D55" s="11"/>
+      <c r="E55" s="11"/>
+      <c r="F55" s="11"/>
+      <c r="G55" s="27"/>
+      <c r="H55" s="27"/>
+      <c r="I55" s="11"/>
+      <c r="J55" s="27"/>
       <c r="K55" s="1"/>
       <c r="L55" s="1"/>
       <c r="M55" s="1"/>
@@ -2744,15 +2744,15 @@
       <c r="A56" s="7">
         <v>48</v>
       </c>
-      <c r="B56" s="13"/>
-      <c r="C56" s="13"/>
-      <c r="D56" s="13"/>
-      <c r="E56" s="13"/>
-      <c r="F56" s="13"/>
-      <c r="G56" s="29"/>
-      <c r="H56" s="29"/>
-      <c r="I56" s="13"/>
-      <c r="J56" s="29"/>
+      <c r="B56" s="11"/>
+      <c r="C56" s="11"/>
+      <c r="D56" s="11"/>
+      <c r="E56" s="11"/>
+      <c r="F56" s="11"/>
+      <c r="G56" s="27"/>
+      <c r="H56" s="27"/>
+      <c r="I56" s="11"/>
+      <c r="J56" s="27"/>
       <c r="K56" s="1"/>
       <c r="L56" s="1"/>
       <c r="M56" s="1"/>
@@ -2777,15 +2777,15 @@
       <c r="A57" s="7">
         <v>49</v>
       </c>
-      <c r="B57" s="13"/>
-      <c r="C57" s="13"/>
-      <c r="D57" s="13"/>
-      <c r="E57" s="13"/>
-      <c r="F57" s="13"/>
-      <c r="G57" s="29"/>
-      <c r="H57" s="29"/>
-      <c r="I57" s="13"/>
-      <c r="J57" s="29"/>
+      <c r="B57" s="11"/>
+      <c r="C57" s="11"/>
+      <c r="D57" s="11"/>
+      <c r="E57" s="11"/>
+      <c r="F57" s="11"/>
+      <c r="G57" s="27"/>
+      <c r="H57" s="27"/>
+      <c r="I57" s="11"/>
+      <c r="J57" s="27"/>
       <c r="K57" s="1"/>
       <c r="L57" s="1"/>
       <c r="M57" s="1"/>
@@ -2810,15 +2810,15 @@
       <c r="A58" s="7">
         <v>50</v>
       </c>
-      <c r="B58" s="13"/>
-      <c r="C58" s="13"/>
-      <c r="D58" s="13"/>
-      <c r="E58" s="13"/>
-      <c r="F58" s="13"/>
-      <c r="G58" s="29"/>
-      <c r="H58" s="29"/>
-      <c r="I58" s="13"/>
-      <c r="J58" s="29"/>
+      <c r="B58" s="11"/>
+      <c r="C58" s="11"/>
+      <c r="D58" s="11"/>
+      <c r="E58" s="11"/>
+      <c r="F58" s="11"/>
+      <c r="G58" s="27"/>
+      <c r="H58" s="27"/>
+      <c r="I58" s="11"/>
+      <c r="J58" s="27"/>
       <c r="K58" s="1"/>
       <c r="L58" s="1"/>
       <c r="M58" s="1"/>
@@ -2843,15 +2843,15 @@
       <c r="A59" s="7">
         <v>51</v>
       </c>
-      <c r="B59" s="13"/>
-      <c r="C59" s="13"/>
-      <c r="D59" s="13"/>
-      <c r="E59" s="13"/>
-      <c r="F59" s="13"/>
-      <c r="G59" s="29"/>
-      <c r="H59" s="29"/>
-      <c r="I59" s="13"/>
-      <c r="J59" s="29"/>
+      <c r="B59" s="11"/>
+      <c r="C59" s="11"/>
+      <c r="D59" s="11"/>
+      <c r="E59" s="11"/>
+      <c r="F59" s="11"/>
+      <c r="G59" s="27"/>
+      <c r="H59" s="27"/>
+      <c r="I59" s="11"/>
+      <c r="J59" s="27"/>
       <c r="K59" s="1"/>
       <c r="L59" s="1"/>
       <c r="M59" s="1"/>
@@ -2876,15 +2876,15 @@
       <c r="A60" s="7">
         <v>52</v>
       </c>
-      <c r="B60" s="13"/>
-      <c r="C60" s="13"/>
-      <c r="D60" s="13"/>
-      <c r="E60" s="13"/>
-      <c r="F60" s="13"/>
-      <c r="G60" s="29"/>
-      <c r="H60" s="29"/>
-      <c r="I60" s="13"/>
-      <c r="J60" s="29"/>
+      <c r="B60" s="11"/>
+      <c r="C60" s="11"/>
+      <c r="D60" s="11"/>
+      <c r="E60" s="11"/>
+      <c r="F60" s="11"/>
+      <c r="G60" s="27"/>
+      <c r="H60" s="27"/>
+      <c r="I60" s="11"/>
+      <c r="J60" s="27"/>
       <c r="K60" s="1"/>
       <c r="L60" s="1"/>
       <c r="M60" s="1"/>
@@ -2909,15 +2909,15 @@
       <c r="A61" s="7">
         <v>53</v>
       </c>
-      <c r="B61" s="13"/>
-      <c r="C61" s="13"/>
-      <c r="D61" s="13"/>
-      <c r="E61" s="13"/>
-      <c r="F61" s="13"/>
-      <c r="G61" s="29"/>
-      <c r="H61" s="29"/>
-      <c r="I61" s="13"/>
-      <c r="J61" s="29"/>
+      <c r="B61" s="11"/>
+      <c r="C61" s="11"/>
+      <c r="D61" s="11"/>
+      <c r="E61" s="11"/>
+      <c r="F61" s="11"/>
+      <c r="G61" s="27"/>
+      <c r="H61" s="27"/>
+      <c r="I61" s="11"/>
+      <c r="J61" s="27"/>
       <c r="K61" s="1"/>
       <c r="L61" s="1"/>
       <c r="M61" s="1"/>
@@ -2942,15 +2942,15 @@
       <c r="A62" s="7">
         <v>54</v>
       </c>
-      <c r="B62" s="13"/>
-      <c r="C62" s="13"/>
-      <c r="D62" s="13"/>
-      <c r="E62" s="13"/>
-      <c r="F62" s="13"/>
-      <c r="G62" s="29"/>
-      <c r="H62" s="29"/>
-      <c r="I62" s="13"/>
-      <c r="J62" s="29"/>
+      <c r="B62" s="11"/>
+      <c r="C62" s="11"/>
+      <c r="D62" s="11"/>
+      <c r="E62" s="11"/>
+      <c r="F62" s="11"/>
+      <c r="G62" s="27"/>
+      <c r="H62" s="27"/>
+      <c r="I62" s="11"/>
+      <c r="J62" s="27"/>
       <c r="K62" s="1"/>
       <c r="L62" s="1"/>
       <c r="M62" s="1"/>
@@ -2975,15 +2975,15 @@
       <c r="A63" s="7">
         <v>55</v>
       </c>
-      <c r="B63" s="13"/>
-      <c r="C63" s="13"/>
-      <c r="D63" s="13"/>
-      <c r="E63" s="13"/>
-      <c r="F63" s="13"/>
-      <c r="G63" s="29"/>
-      <c r="H63" s="29"/>
-      <c r="I63" s="13"/>
-      <c r="J63" s="29"/>
+      <c r="B63" s="11"/>
+      <c r="C63" s="11"/>
+      <c r="D63" s="11"/>
+      <c r="E63" s="11"/>
+      <c r="F63" s="11"/>
+      <c r="G63" s="27"/>
+      <c r="H63" s="27"/>
+      <c r="I63" s="11"/>
+      <c r="J63" s="27"/>
       <c r="K63" s="1"/>
       <c r="L63" s="1"/>
       <c r="M63" s="1"/>
@@ -3008,15 +3008,15 @@
       <c r="A64" s="7">
         <v>56</v>
       </c>
-      <c r="B64" s="13"/>
-      <c r="C64" s="13"/>
-      <c r="D64" s="13"/>
-      <c r="E64" s="13"/>
-      <c r="F64" s="13"/>
-      <c r="G64" s="29"/>
-      <c r="H64" s="29"/>
-      <c r="I64" s="13"/>
-      <c r="J64" s="29"/>
+      <c r="B64" s="11"/>
+      <c r="C64" s="11"/>
+      <c r="D64" s="11"/>
+      <c r="E64" s="11"/>
+      <c r="F64" s="11"/>
+      <c r="G64" s="27"/>
+      <c r="H64" s="27"/>
+      <c r="I64" s="11"/>
+      <c r="J64" s="27"/>
       <c r="K64" s="1"/>
       <c r="L64" s="1"/>
       <c r="M64" s="1"/>
@@ -3041,15 +3041,15 @@
       <c r="A65" s="7">
         <v>57</v>
       </c>
-      <c r="B65" s="13"/>
-      <c r="C65" s="13"/>
-      <c r="D65" s="13"/>
-      <c r="E65" s="13"/>
-      <c r="F65" s="13"/>
-      <c r="G65" s="29"/>
-      <c r="H65" s="29"/>
-      <c r="I65" s="13"/>
-      <c r="J65" s="29"/>
+      <c r="B65" s="11"/>
+      <c r="C65" s="11"/>
+      <c r="D65" s="11"/>
+      <c r="E65" s="11"/>
+      <c r="F65" s="11"/>
+      <c r="G65" s="27"/>
+      <c r="H65" s="27"/>
+      <c r="I65" s="11"/>
+      <c r="J65" s="27"/>
       <c r="K65" s="1"/>
       <c r="L65" s="1"/>
       <c r="M65" s="1"/>
@@ -3074,15 +3074,15 @@
       <c r="A66" s="7">
         <v>58</v>
       </c>
-      <c r="B66" s="13"/>
-      <c r="C66" s="13"/>
-      <c r="D66" s="13"/>
-      <c r="E66" s="13"/>
-      <c r="F66" s="13"/>
-      <c r="G66" s="29"/>
-      <c r="H66" s="29"/>
-      <c r="I66" s="13"/>
-      <c r="J66" s="29"/>
+      <c r="B66" s="11"/>
+      <c r="C66" s="11"/>
+      <c r="D66" s="11"/>
+      <c r="E66" s="11"/>
+      <c r="F66" s="11"/>
+      <c r="G66" s="27"/>
+      <c r="H66" s="27"/>
+      <c r="I66" s="11"/>
+      <c r="J66" s="27"/>
       <c r="K66" s="1"/>
       <c r="L66" s="1"/>
       <c r="M66" s="1"/>
@@ -3107,15 +3107,15 @@
       <c r="A67" s="7">
         <v>59</v>
       </c>
-      <c r="B67" s="13"/>
-      <c r="C67" s="13"/>
-      <c r="D67" s="13"/>
-      <c r="E67" s="13"/>
-      <c r="F67" s="13"/>
-      <c r="G67" s="29"/>
-      <c r="H67" s="29"/>
-      <c r="I67" s="13"/>
-      <c r="J67" s="29"/>
+      <c r="B67" s="11"/>
+      <c r="C67" s="11"/>
+      <c r="D67" s="11"/>
+      <c r="E67" s="11"/>
+      <c r="F67" s="11"/>
+      <c r="G67" s="27"/>
+      <c r="H67" s="27"/>
+      <c r="I67" s="11"/>
+      <c r="J67" s="27"/>
       <c r="K67" s="1"/>
       <c r="L67" s="1"/>
       <c r="M67" s="1"/>
@@ -3140,15 +3140,15 @@
       <c r="A68" s="7">
         <v>60</v>
       </c>
-      <c r="B68" s="13"/>
-      <c r="C68" s="13"/>
-      <c r="D68" s="13"/>
-      <c r="E68" s="13"/>
-      <c r="F68" s="13"/>
-      <c r="G68" s="29"/>
-      <c r="H68" s="29"/>
-      <c r="I68" s="13"/>
-      <c r="J68" s="29"/>
+      <c r="B68" s="11"/>
+      <c r="C68" s="11"/>
+      <c r="D68" s="11"/>
+      <c r="E68" s="11"/>
+      <c r="F68" s="11"/>
+      <c r="G68" s="27"/>
+      <c r="H68" s="27"/>
+      <c r="I68" s="11"/>
+      <c r="J68" s="27"/>
       <c r="K68" s="1"/>
       <c r="L68" s="1"/>
       <c r="M68" s="1"/>
@@ -3173,15 +3173,15 @@
       <c r="A69" s="7">
         <v>61</v>
       </c>
-      <c r="B69" s="13"/>
-      <c r="C69" s="13"/>
-      <c r="D69" s="13"/>
-      <c r="E69" s="13"/>
-      <c r="F69" s="13"/>
-      <c r="G69" s="29"/>
-      <c r="H69" s="29"/>
-      <c r="I69" s="13"/>
-      <c r="J69" s="29"/>
+      <c r="B69" s="11"/>
+      <c r="C69" s="11"/>
+      <c r="D69" s="11"/>
+      <c r="E69" s="11"/>
+      <c r="F69" s="11"/>
+      <c r="G69" s="27"/>
+      <c r="H69" s="27"/>
+      <c r="I69" s="11"/>
+      <c r="J69" s="27"/>
       <c r="K69" s="1"/>
       <c r="L69" s="1"/>
       <c r="M69" s="1"/>
@@ -3206,15 +3206,15 @@
       <c r="A70" s="7">
         <v>62</v>
       </c>
-      <c r="B70" s="13"/>
-      <c r="C70" s="13"/>
-      <c r="D70" s="13"/>
-      <c r="E70" s="13"/>
-      <c r="F70" s="13"/>
-      <c r="G70" s="29"/>
-      <c r="H70" s="29"/>
-      <c r="I70" s="13"/>
-      <c r="J70" s="29"/>
+      <c r="B70" s="11"/>
+      <c r="C70" s="11"/>
+      <c r="D70" s="11"/>
+      <c r="E70" s="11"/>
+      <c r="F70" s="11"/>
+      <c r="G70" s="27"/>
+      <c r="H70" s="27"/>
+      <c r="I70" s="11"/>
+      <c r="J70" s="27"/>
       <c r="K70" s="1"/>
       <c r="L70" s="1"/>
       <c r="M70" s="1"/>
@@ -3239,15 +3239,15 @@
       <c r="A71" s="7">
         <v>63</v>
       </c>
-      <c r="B71" s="13"/>
-      <c r="C71" s="13"/>
-      <c r="D71" s="13"/>
-      <c r="E71" s="13"/>
-      <c r="F71" s="13"/>
-      <c r="G71" s="29"/>
-      <c r="H71" s="29"/>
-      <c r="I71" s="13"/>
-      <c r="J71" s="29"/>
+      <c r="B71" s="11"/>
+      <c r="C71" s="11"/>
+      <c r="D71" s="11"/>
+      <c r="E71" s="11"/>
+      <c r="F71" s="11"/>
+      <c r="G71" s="27"/>
+      <c r="H71" s="27"/>
+      <c r="I71" s="11"/>
+      <c r="J71" s="27"/>
       <c r="K71" s="1"/>
       <c r="L71" s="1"/>
       <c r="M71" s="1"/>
@@ -3272,15 +3272,15 @@
       <c r="A72" s="7">
         <v>64</v>
       </c>
-      <c r="B72" s="13"/>
-      <c r="C72" s="13"/>
-      <c r="D72" s="13"/>
-      <c r="E72" s="13"/>
-      <c r="F72" s="13"/>
-      <c r="G72" s="29"/>
-      <c r="H72" s="29"/>
-      <c r="I72" s="13"/>
-      <c r="J72" s="29"/>
+      <c r="B72" s="11"/>
+      <c r="C72" s="11"/>
+      <c r="D72" s="11"/>
+      <c r="E72" s="11"/>
+      <c r="F72" s="11"/>
+      <c r="G72" s="27"/>
+      <c r="H72" s="27"/>
+      <c r="I72" s="11"/>
+      <c r="J72" s="27"/>
       <c r="K72" s="1"/>
       <c r="L72" s="1"/>
       <c r="M72" s="1"/>
@@ -3305,15 +3305,15 @@
       <c r="A73" s="7">
         <v>65</v>
       </c>
-      <c r="B73" s="13"/>
-      <c r="C73" s="13"/>
-      <c r="D73" s="13"/>
-      <c r="E73" s="13"/>
-      <c r="F73" s="13"/>
-      <c r="G73" s="29"/>
-      <c r="H73" s="29"/>
-      <c r="I73" s="13"/>
-      <c r="J73" s="29"/>
+      <c r="B73" s="11"/>
+      <c r="C73" s="11"/>
+      <c r="D73" s="11"/>
+      <c r="E73" s="11"/>
+      <c r="F73" s="11"/>
+      <c r="G73" s="27"/>
+      <c r="H73" s="27"/>
+      <c r="I73" s="11"/>
+      <c r="J73" s="27"/>
       <c r="K73" s="1"/>
       <c r="L73" s="1"/>
       <c r="M73" s="1"/>
@@ -3338,15 +3338,15 @@
       <c r="A74" s="7">
         <v>66</v>
       </c>
-      <c r="B74" s="13"/>
-      <c r="C74" s="13"/>
-      <c r="D74" s="13"/>
-      <c r="E74" s="13"/>
-      <c r="F74" s="13"/>
-      <c r="G74" s="29"/>
-      <c r="H74" s="29"/>
-      <c r="I74" s="13"/>
-      <c r="J74" s="29"/>
+      <c r="B74" s="11"/>
+      <c r="C74" s="11"/>
+      <c r="D74" s="11"/>
+      <c r="E74" s="11"/>
+      <c r="F74" s="11"/>
+      <c r="G74" s="27"/>
+      <c r="H74" s="27"/>
+      <c r="I74" s="11"/>
+      <c r="J74" s="27"/>
       <c r="K74" s="1"/>
       <c r="L74" s="1"/>
       <c r="M74" s="1"/>
@@ -3371,15 +3371,15 @@
       <c r="A75" s="7">
         <v>67</v>
       </c>
-      <c r="B75" s="13"/>
-      <c r="C75" s="13"/>
-      <c r="D75" s="13"/>
-      <c r="E75" s="13"/>
-      <c r="F75" s="13"/>
-      <c r="G75" s="29"/>
-      <c r="H75" s="29"/>
-      <c r="I75" s="13"/>
-      <c r="J75" s="29"/>
+      <c r="B75" s="11"/>
+      <c r="C75" s="11"/>
+      <c r="D75" s="11"/>
+      <c r="E75" s="11"/>
+      <c r="F75" s="11"/>
+      <c r="G75" s="27"/>
+      <c r="H75" s="27"/>
+      <c r="I75" s="11"/>
+      <c r="J75" s="27"/>
       <c r="K75" s="1"/>
       <c r="L75" s="1"/>
       <c r="M75" s="1"/>
@@ -3404,15 +3404,15 @@
       <c r="A76" s="7">
         <v>68</v>
       </c>
-      <c r="B76" s="13"/>
-      <c r="C76" s="13"/>
-      <c r="D76" s="13"/>
-      <c r="E76" s="13"/>
-      <c r="F76" s="13"/>
-      <c r="G76" s="29"/>
-      <c r="H76" s="29"/>
-      <c r="I76" s="13"/>
-      <c r="J76" s="29"/>
+      <c r="B76" s="11"/>
+      <c r="C76" s="11"/>
+      <c r="D76" s="11"/>
+      <c r="E76" s="11"/>
+      <c r="F76" s="11"/>
+      <c r="G76" s="27"/>
+      <c r="H76" s="27"/>
+      <c r="I76" s="11"/>
+      <c r="J76" s="27"/>
       <c r="K76" s="1"/>
       <c r="L76" s="1"/>
       <c r="M76" s="1"/>
@@ -3437,15 +3437,15 @@
       <c r="A77" s="7">
         <v>69</v>
       </c>
-      <c r="B77" s="13"/>
-      <c r="C77" s="13"/>
-      <c r="D77" s="13"/>
-      <c r="E77" s="13"/>
-      <c r="F77" s="13"/>
-      <c r="G77" s="29"/>
-      <c r="H77" s="29"/>
-      <c r="I77" s="13"/>
-      <c r="J77" s="29"/>
+      <c r="B77" s="11"/>
+      <c r="C77" s="11"/>
+      <c r="D77" s="11"/>
+      <c r="E77" s="11"/>
+      <c r="F77" s="11"/>
+      <c r="G77" s="27"/>
+      <c r="H77" s="27"/>
+      <c r="I77" s="11"/>
+      <c r="J77" s="27"/>
       <c r="K77" s="1"/>
       <c r="L77" s="1"/>
       <c r="M77" s="1"/>
@@ -3470,15 +3470,15 @@
       <c r="A78" s="7">
         <v>70</v>
       </c>
-      <c r="B78" s="13"/>
-      <c r="C78" s="13"/>
-      <c r="D78" s="13"/>
-      <c r="E78" s="13"/>
-      <c r="F78" s="13"/>
-      <c r="G78" s="29"/>
-      <c r="H78" s="29"/>
-      <c r="I78" s="13"/>
-      <c r="J78" s="29"/>
+      <c r="B78" s="11"/>
+      <c r="C78" s="11"/>
+      <c r="D78" s="11"/>
+      <c r="E78" s="11"/>
+      <c r="F78" s="11"/>
+      <c r="G78" s="27"/>
+      <c r="H78" s="27"/>
+      <c r="I78" s="11"/>
+      <c r="J78" s="27"/>
       <c r="K78" s="1"/>
       <c r="L78" s="1"/>
       <c r="M78" s="1"/>
@@ -3500,700 +3500,700 @@
       <c r="AC78" s="1"/>
     </row>
     <row r="79" spans="1:29" ht="15">
-      <c r="G79" s="29"/>
-      <c r="H79" s="29"/>
-      <c r="I79" s="13"/>
-      <c r="J79" s="29"/>
+      <c r="G79" s="27"/>
+      <c r="H79" s="27"/>
+      <c r="I79" s="11"/>
+      <c r="J79" s="27"/>
     </row>
     <row r="80" spans="1:29" ht="15">
-      <c r="G80" s="29"/>
-      <c r="H80" s="29"/>
-      <c r="I80" s="13"/>
-      <c r="J80" s="29"/>
+      <c r="G80" s="27"/>
+      <c r="H80" s="27"/>
+      <c r="I80" s="11"/>
+      <c r="J80" s="27"/>
     </row>
     <row r="81" spans="7:10" ht="15">
-      <c r="G81" s="29"/>
-      <c r="H81" s="29"/>
-      <c r="I81" s="13"/>
-      <c r="J81" s="29"/>
+      <c r="G81" s="27"/>
+      <c r="H81" s="27"/>
+      <c r="I81" s="11"/>
+      <c r="J81" s="27"/>
     </row>
     <row r="82" spans="7:10" ht="15">
-      <c r="G82" s="29"/>
-      <c r="H82" s="29"/>
-      <c r="I82" s="13"/>
-      <c r="J82" s="29"/>
+      <c r="G82" s="27"/>
+      <c r="H82" s="27"/>
+      <c r="I82" s="11"/>
+      <c r="J82" s="27"/>
     </row>
     <row r="83" spans="7:10" ht="15">
-      <c r="G83" s="29"/>
-      <c r="H83" s="29"/>
-      <c r="I83" s="13"/>
-      <c r="J83" s="29"/>
+      <c r="G83" s="27"/>
+      <c r="H83" s="27"/>
+      <c r="I83" s="11"/>
+      <c r="J83" s="27"/>
     </row>
     <row r="84" spans="7:10" ht="15">
-      <c r="G84" s="29"/>
-      <c r="H84" s="29"/>
-      <c r="I84" s="13"/>
-      <c r="J84" s="29"/>
+      <c r="G84" s="27"/>
+      <c r="H84" s="27"/>
+      <c r="I84" s="11"/>
+      <c r="J84" s="27"/>
     </row>
     <row r="85" spans="7:10" ht="15">
-      <c r="G85" s="30"/>
-      <c r="H85" s="30"/>
-      <c r="I85" s="13"/>
-      <c r="J85" s="29"/>
+      <c r="G85" s="28"/>
+      <c r="H85" s="28"/>
+      <c r="I85" s="11"/>
+      <c r="J85" s="27"/>
     </row>
     <row r="86" spans="7:10" ht="15">
-      <c r="G86" s="30"/>
-      <c r="H86" s="30"/>
-      <c r="I86" s="13"/>
-      <c r="J86" s="29"/>
+      <c r="G86" s="28"/>
+      <c r="H86" s="28"/>
+      <c r="I86" s="11"/>
+      <c r="J86" s="27"/>
     </row>
     <row r="87" spans="7:10" ht="15">
-      <c r="G87" s="30"/>
-      <c r="H87" s="30"/>
-      <c r="I87" s="13"/>
-      <c r="J87" s="29"/>
+      <c r="G87" s="28"/>
+      <c r="H87" s="28"/>
+      <c r="I87" s="11"/>
+      <c r="J87" s="27"/>
     </row>
     <row r="88" spans="7:10" ht="15">
-      <c r="G88" s="30"/>
-      <c r="H88" s="30"/>
-      <c r="I88" s="13"/>
-      <c r="J88" s="29"/>
+      <c r="G88" s="28"/>
+      <c r="H88" s="28"/>
+      <c r="I88" s="11"/>
+      <c r="J88" s="27"/>
     </row>
     <row r="89" spans="7:10" ht="15">
-      <c r="G89" s="30"/>
-      <c r="H89" s="30"/>
-      <c r="I89" s="13"/>
-      <c r="J89" s="29"/>
+      <c r="G89" s="28"/>
+      <c r="H89" s="28"/>
+      <c r="I89" s="11"/>
+      <c r="J89" s="27"/>
     </row>
     <row r="90" spans="7:10" ht="15">
-      <c r="G90" s="30"/>
-      <c r="H90" s="30"/>
-      <c r="I90" s="13"/>
-      <c r="J90" s="29"/>
+      <c r="G90" s="28"/>
+      <c r="H90" s="28"/>
+      <c r="I90" s="11"/>
+      <c r="J90" s="27"/>
     </row>
     <row r="91" spans="7:10">
-      <c r="G91" s="30"/>
-      <c r="H91" s="30"/>
+      <c r="G91" s="28"/>
+      <c r="H91" s="28"/>
     </row>
     <row r="92" spans="7:10">
-      <c r="G92" s="30"/>
-      <c r="H92" s="30"/>
+      <c r="G92" s="28"/>
+      <c r="H92" s="28"/>
     </row>
     <row r="93" spans="7:10">
-      <c r="G93" s="30"/>
-      <c r="H93" s="30"/>
+      <c r="G93" s="28"/>
+      <c r="H93" s="28"/>
     </row>
     <row r="94" spans="7:10">
-      <c r="G94" s="30"/>
-      <c r="H94" s="30"/>
+      <c r="G94" s="28"/>
+      <c r="H94" s="28"/>
     </row>
     <row r="95" spans="7:10">
-      <c r="G95" s="30"/>
-      <c r="H95" s="30"/>
+      <c r="G95" s="28"/>
+      <c r="H95" s="28"/>
     </row>
     <row r="96" spans="7:10">
-      <c r="G96" s="30"/>
-      <c r="H96" s="30"/>
+      <c r="G96" s="28"/>
+      <c r="H96" s="28"/>
     </row>
     <row r="97" spans="7:8">
-      <c r="G97" s="30"/>
-      <c r="H97" s="30"/>
+      <c r="G97" s="28"/>
+      <c r="H97" s="28"/>
     </row>
     <row r="98" spans="7:8">
-      <c r="G98" s="30"/>
-      <c r="H98" s="30"/>
+      <c r="G98" s="28"/>
+      <c r="H98" s="28"/>
     </row>
     <row r="99" spans="7:8">
-      <c r="G99" s="30"/>
-      <c r="H99" s="30"/>
+      <c r="G99" s="28"/>
+      <c r="H99" s="28"/>
     </row>
     <row r="100" spans="7:8">
-      <c r="G100" s="30"/>
-      <c r="H100" s="30"/>
+      <c r="G100" s="28"/>
+      <c r="H100" s="28"/>
     </row>
     <row r="101" spans="7:8">
-      <c r="G101" s="30"/>
-      <c r="H101" s="30"/>
+      <c r="G101" s="28"/>
+      <c r="H101" s="28"/>
     </row>
     <row r="102" spans="7:8">
-      <c r="G102" s="30"/>
-      <c r="H102" s="30"/>
+      <c r="G102" s="28"/>
+      <c r="H102" s="28"/>
     </row>
     <row r="103" spans="7:8">
-      <c r="G103" s="30"/>
-      <c r="H103" s="30"/>
+      <c r="G103" s="28"/>
+      <c r="H103" s="28"/>
     </row>
     <row r="104" spans="7:8">
-      <c r="G104" s="30"/>
-      <c r="H104" s="30"/>
+      <c r="G104" s="28"/>
+      <c r="H104" s="28"/>
     </row>
     <row r="105" spans="7:8">
-      <c r="G105" s="30"/>
-      <c r="H105" s="30"/>
+      <c r="G105" s="28"/>
+      <c r="H105" s="28"/>
     </row>
     <row r="106" spans="7:8">
-      <c r="G106" s="30"/>
-      <c r="H106" s="30"/>
+      <c r="G106" s="28"/>
+      <c r="H106" s="28"/>
     </row>
     <row r="107" spans="7:8">
-      <c r="G107" s="30"/>
-      <c r="H107" s="30"/>
+      <c r="G107" s="28"/>
+      <c r="H107" s="28"/>
     </row>
     <row r="108" spans="7:8">
-      <c r="G108" s="30"/>
-      <c r="H108" s="30"/>
+      <c r="G108" s="28"/>
+      <c r="H108" s="28"/>
     </row>
     <row r="109" spans="7:8">
-      <c r="G109" s="30"/>
-      <c r="H109" s="30"/>
+      <c r="G109" s="28"/>
+      <c r="H109" s="28"/>
     </row>
     <row r="110" spans="7:8">
-      <c r="G110" s="30"/>
-      <c r="H110" s="30"/>
+      <c r="G110" s="28"/>
+      <c r="H110" s="28"/>
     </row>
     <row r="111" spans="7:8">
-      <c r="G111" s="30"/>
-      <c r="H111" s="30"/>
+      <c r="G111" s="28"/>
+      <c r="H111" s="28"/>
     </row>
     <row r="112" spans="7:8">
-      <c r="G112" s="30"/>
-      <c r="H112" s="30"/>
+      <c r="G112" s="28"/>
+      <c r="H112" s="28"/>
     </row>
     <row r="113" spans="7:8">
-      <c r="G113" s="30"/>
-      <c r="H113" s="30"/>
+      <c r="G113" s="28"/>
+      <c r="H113" s="28"/>
     </row>
     <row r="114" spans="7:8">
-      <c r="G114" s="30"/>
-      <c r="H114" s="30"/>
+      <c r="G114" s="28"/>
+      <c r="H114" s="28"/>
     </row>
     <row r="115" spans="7:8">
-      <c r="G115" s="30"/>
-      <c r="H115" s="30"/>
+      <c r="G115" s="28"/>
+      <c r="H115" s="28"/>
     </row>
     <row r="116" spans="7:8">
-      <c r="G116" s="30"/>
-      <c r="H116" s="30"/>
+      <c r="G116" s="28"/>
+      <c r="H116" s="28"/>
     </row>
     <row r="117" spans="7:8">
-      <c r="G117" s="30"/>
-      <c r="H117" s="30"/>
+      <c r="G117" s="28"/>
+      <c r="H117" s="28"/>
     </row>
     <row r="118" spans="7:8">
-      <c r="G118" s="30"/>
-      <c r="H118" s="30"/>
+      <c r="G118" s="28"/>
+      <c r="H118" s="28"/>
     </row>
     <row r="119" spans="7:8">
-      <c r="G119" s="30"/>
-      <c r="H119" s="30"/>
+      <c r="G119" s="28"/>
+      <c r="H119" s="28"/>
     </row>
     <row r="120" spans="7:8">
-      <c r="G120" s="30"/>
-      <c r="H120" s="30"/>
+      <c r="G120" s="28"/>
+      <c r="H120" s="28"/>
     </row>
     <row r="121" spans="7:8">
-      <c r="G121" s="30"/>
-      <c r="H121" s="30"/>
+      <c r="G121" s="28"/>
+      <c r="H121" s="28"/>
     </row>
     <row r="122" spans="7:8">
-      <c r="G122" s="30"/>
-      <c r="H122" s="30"/>
+      <c r="G122" s="28"/>
+      <c r="H122" s="28"/>
     </row>
     <row r="123" spans="7:8">
-      <c r="G123" s="30"/>
-      <c r="H123" s="30"/>
+      <c r="G123" s="28"/>
+      <c r="H123" s="28"/>
     </row>
     <row r="124" spans="7:8">
-      <c r="G124" s="30"/>
-      <c r="H124" s="30"/>
+      <c r="G124" s="28"/>
+      <c r="H124" s="28"/>
     </row>
     <row r="125" spans="7:8">
-      <c r="G125" s="30"/>
-      <c r="H125" s="30"/>
+      <c r="G125" s="28"/>
+      <c r="H125" s="28"/>
     </row>
     <row r="126" spans="7:8">
-      <c r="G126" s="30"/>
-      <c r="H126" s="30"/>
+      <c r="G126" s="28"/>
+      <c r="H126" s="28"/>
     </row>
     <row r="127" spans="7:8">
-      <c r="G127" s="30"/>
-      <c r="H127" s="30"/>
+      <c r="G127" s="28"/>
+      <c r="H127" s="28"/>
     </row>
     <row r="128" spans="7:8">
-      <c r="G128" s="30"/>
-      <c r="H128" s="30"/>
+      <c r="G128" s="28"/>
+      <c r="H128" s="28"/>
     </row>
     <row r="129" spans="7:8">
-      <c r="G129" s="30"/>
-      <c r="H129" s="30"/>
+      <c r="G129" s="28"/>
+      <c r="H129" s="28"/>
     </row>
     <row r="130" spans="7:8">
-      <c r="G130" s="30"/>
-      <c r="H130" s="30"/>
+      <c r="G130" s="28"/>
+      <c r="H130" s="28"/>
     </row>
     <row r="131" spans="7:8">
-      <c r="G131" s="30"/>
-      <c r="H131" s="30"/>
+      <c r="G131" s="28"/>
+      <c r="H131" s="28"/>
     </row>
     <row r="132" spans="7:8">
-      <c r="G132" s="30"/>
-      <c r="H132" s="30"/>
+      <c r="G132" s="28"/>
+      <c r="H132" s="28"/>
     </row>
     <row r="133" spans="7:8">
-      <c r="G133" s="30"/>
-      <c r="H133" s="30"/>
+      <c r="G133" s="28"/>
+      <c r="H133" s="28"/>
     </row>
     <row r="134" spans="7:8">
-      <c r="G134" s="30"/>
-      <c r="H134" s="30"/>
+      <c r="G134" s="28"/>
+      <c r="H134" s="28"/>
     </row>
     <row r="135" spans="7:8">
-      <c r="G135" s="30"/>
-      <c r="H135" s="30"/>
+      <c r="G135" s="28"/>
+      <c r="H135" s="28"/>
     </row>
     <row r="136" spans="7:8">
-      <c r="G136" s="30"/>
-      <c r="H136" s="30"/>
+      <c r="G136" s="28"/>
+      <c r="H136" s="28"/>
     </row>
     <row r="137" spans="7:8">
-      <c r="G137" s="30"/>
-      <c r="H137" s="30"/>
+      <c r="G137" s="28"/>
+      <c r="H137" s="28"/>
     </row>
     <row r="138" spans="7:8">
-      <c r="G138" s="30"/>
-      <c r="H138" s="30"/>
+      <c r="G138" s="28"/>
+      <c r="H138" s="28"/>
     </row>
     <row r="139" spans="7:8">
-      <c r="G139" s="30"/>
-      <c r="H139" s="30"/>
+      <c r="G139" s="28"/>
+      <c r="H139" s="28"/>
     </row>
     <row r="140" spans="7:8">
-      <c r="G140" s="30"/>
-      <c r="H140" s="30"/>
+      <c r="G140" s="28"/>
+      <c r="H140" s="28"/>
     </row>
     <row r="141" spans="7:8">
-      <c r="G141" s="30"/>
-      <c r="H141" s="30"/>
+      <c r="G141" s="28"/>
+      <c r="H141" s="28"/>
     </row>
     <row r="142" spans="7:8">
-      <c r="G142" s="30"/>
-      <c r="H142" s="30"/>
+      <c r="G142" s="28"/>
+      <c r="H142" s="28"/>
     </row>
     <row r="143" spans="7:8">
-      <c r="G143" s="30"/>
-      <c r="H143" s="30"/>
+      <c r="G143" s="28"/>
+      <c r="H143" s="28"/>
     </row>
     <row r="144" spans="7:8">
-      <c r="G144" s="30"/>
-      <c r="H144" s="30"/>
+      <c r="G144" s="28"/>
+      <c r="H144" s="28"/>
     </row>
     <row r="145" spans="7:8">
-      <c r="G145" s="30"/>
-      <c r="H145" s="30"/>
+      <c r="G145" s="28"/>
+      <c r="H145" s="28"/>
     </row>
     <row r="146" spans="7:8">
-      <c r="G146" s="30"/>
-      <c r="H146" s="30"/>
+      <c r="G146" s="28"/>
+      <c r="H146" s="28"/>
     </row>
     <row r="147" spans="7:8">
-      <c r="G147" s="30"/>
-      <c r="H147" s="30"/>
+      <c r="G147" s="28"/>
+      <c r="H147" s="28"/>
     </row>
     <row r="148" spans="7:8">
-      <c r="G148" s="30"/>
-      <c r="H148" s="30"/>
+      <c r="G148" s="28"/>
+      <c r="H148" s="28"/>
     </row>
     <row r="149" spans="7:8">
-      <c r="G149" s="30"/>
-      <c r="H149" s="30"/>
+      <c r="G149" s="28"/>
+      <c r="H149" s="28"/>
     </row>
     <row r="150" spans="7:8">
-      <c r="G150" s="30"/>
-      <c r="H150" s="30"/>
+      <c r="G150" s="28"/>
+      <c r="H150" s="28"/>
     </row>
     <row r="151" spans="7:8">
-      <c r="G151" s="30"/>
-      <c r="H151" s="30"/>
+      <c r="G151" s="28"/>
+      <c r="H151" s="28"/>
     </row>
     <row r="152" spans="7:8">
-      <c r="G152" s="30"/>
-      <c r="H152" s="30"/>
+      <c r="G152" s="28"/>
+      <c r="H152" s="28"/>
     </row>
     <row r="153" spans="7:8">
-      <c r="G153" s="30"/>
-      <c r="H153" s="30"/>
+      <c r="G153" s="28"/>
+      <c r="H153" s="28"/>
     </row>
     <row r="154" spans="7:8">
-      <c r="G154" s="30"/>
-      <c r="H154" s="30"/>
+      <c r="G154" s="28"/>
+      <c r="H154" s="28"/>
     </row>
     <row r="155" spans="7:8">
-      <c r="G155" s="30"/>
-      <c r="H155" s="30"/>
+      <c r="G155" s="28"/>
+      <c r="H155" s="28"/>
     </row>
     <row r="156" spans="7:8">
-      <c r="G156" s="30"/>
-      <c r="H156" s="30"/>
+      <c r="G156" s="28"/>
+      <c r="H156" s="28"/>
     </row>
     <row r="157" spans="7:8">
-      <c r="G157" s="30"/>
-      <c r="H157" s="30"/>
+      <c r="G157" s="28"/>
+      <c r="H157" s="28"/>
     </row>
     <row r="158" spans="7:8">
-      <c r="G158" s="30"/>
-      <c r="H158" s="30"/>
+      <c r="G158" s="28"/>
+      <c r="H158" s="28"/>
     </row>
     <row r="159" spans="7:8">
-      <c r="G159" s="30"/>
-      <c r="H159" s="30"/>
+      <c r="G159" s="28"/>
+      <c r="H159" s="28"/>
     </row>
     <row r="160" spans="7:8">
-      <c r="G160" s="30"/>
-      <c r="H160" s="30"/>
+      <c r="G160" s="28"/>
+      <c r="H160" s="28"/>
     </row>
     <row r="161" spans="7:8">
-      <c r="G161" s="30"/>
-      <c r="H161" s="30"/>
+      <c r="G161" s="28"/>
+      <c r="H161" s="28"/>
     </row>
     <row r="162" spans="7:8">
-      <c r="G162" s="30"/>
-      <c r="H162" s="30"/>
+      <c r="G162" s="28"/>
+      <c r="H162" s="28"/>
     </row>
     <row r="163" spans="7:8">
-      <c r="G163" s="30"/>
-      <c r="H163" s="30"/>
+      <c r="G163" s="28"/>
+      <c r="H163" s="28"/>
     </row>
     <row r="164" spans="7:8">
-      <c r="G164" s="30"/>
-      <c r="H164" s="30"/>
+      <c r="G164" s="28"/>
+      <c r="H164" s="28"/>
     </row>
     <row r="165" spans="7:8">
-      <c r="G165" s="30"/>
-      <c r="H165" s="30"/>
+      <c r="G165" s="28"/>
+      <c r="H165" s="28"/>
     </row>
     <row r="166" spans="7:8">
-      <c r="G166" s="30"/>
-      <c r="H166" s="30"/>
+      <c r="G166" s="28"/>
+      <c r="H166" s="28"/>
     </row>
     <row r="167" spans="7:8">
-      <c r="G167" s="30"/>
-      <c r="H167" s="30"/>
+      <c r="G167" s="28"/>
+      <c r="H167" s="28"/>
     </row>
     <row r="168" spans="7:8">
-      <c r="G168" s="30"/>
-      <c r="H168" s="30"/>
+      <c r="G168" s="28"/>
+      <c r="H168" s="28"/>
     </row>
     <row r="169" spans="7:8">
-      <c r="G169" s="30"/>
-      <c r="H169" s="30"/>
+      <c r="G169" s="28"/>
+      <c r="H169" s="28"/>
     </row>
     <row r="170" spans="7:8">
-      <c r="G170" s="30"/>
-      <c r="H170" s="30"/>
+      <c r="G170" s="28"/>
+      <c r="H170" s="28"/>
     </row>
     <row r="171" spans="7:8">
-      <c r="G171" s="30"/>
-      <c r="H171" s="30"/>
+      <c r="G171" s="28"/>
+      <c r="H171" s="28"/>
     </row>
     <row r="172" spans="7:8">
-      <c r="G172" s="30"/>
-      <c r="H172" s="30"/>
+      <c r="G172" s="28"/>
+      <c r="H172" s="28"/>
     </row>
     <row r="173" spans="7:8">
-      <c r="G173" s="30"/>
-      <c r="H173" s="30"/>
+      <c r="G173" s="28"/>
+      <c r="H173" s="28"/>
     </row>
     <row r="174" spans="7:8">
-      <c r="G174" s="30"/>
-      <c r="H174" s="30"/>
+      <c r="G174" s="28"/>
+      <c r="H174" s="28"/>
     </row>
     <row r="175" spans="7:8">
-      <c r="G175" s="30"/>
-      <c r="H175" s="30"/>
+      <c r="G175" s="28"/>
+      <c r="H175" s="28"/>
     </row>
     <row r="176" spans="7:8">
-      <c r="G176" s="30"/>
-      <c r="H176" s="30"/>
+      <c r="G176" s="28"/>
+      <c r="H176" s="28"/>
     </row>
     <row r="177" spans="7:8">
-      <c r="G177" s="30"/>
-      <c r="H177" s="30"/>
+      <c r="G177" s="28"/>
+      <c r="H177" s="28"/>
     </row>
     <row r="178" spans="7:8">
-      <c r="G178" s="30"/>
-      <c r="H178" s="30"/>
+      <c r="G178" s="28"/>
+      <c r="H178" s="28"/>
     </row>
     <row r="179" spans="7:8">
-      <c r="G179" s="30"/>
-      <c r="H179" s="30"/>
+      <c r="G179" s="28"/>
+      <c r="H179" s="28"/>
     </row>
     <row r="180" spans="7:8">
-      <c r="G180" s="30"/>
-      <c r="H180" s="30"/>
+      <c r="G180" s="28"/>
+      <c r="H180" s="28"/>
     </row>
     <row r="181" spans="7:8">
-      <c r="G181" s="30"/>
-      <c r="H181" s="30"/>
+      <c r="G181" s="28"/>
+      <c r="H181" s="28"/>
     </row>
     <row r="182" spans="7:8">
-      <c r="G182" s="30"/>
-      <c r="H182" s="30"/>
+      <c r="G182" s="28"/>
+      <c r="H182" s="28"/>
     </row>
     <row r="183" spans="7:8">
-      <c r="G183" s="30"/>
-      <c r="H183" s="30"/>
+      <c r="G183" s="28"/>
+      <c r="H183" s="28"/>
     </row>
     <row r="184" spans="7:8">
-      <c r="G184" s="30"/>
-      <c r="H184" s="30"/>
+      <c r="G184" s="28"/>
+      <c r="H184" s="28"/>
     </row>
     <row r="185" spans="7:8">
-      <c r="G185" s="30"/>
-      <c r="H185" s="30"/>
+      <c r="G185" s="28"/>
+      <c r="H185" s="28"/>
     </row>
     <row r="186" spans="7:8">
-      <c r="G186" s="30"/>
-      <c r="H186" s="30"/>
+      <c r="G186" s="28"/>
+      <c r="H186" s="28"/>
     </row>
     <row r="187" spans="7:8">
-      <c r="G187" s="30"/>
-      <c r="H187" s="30"/>
+      <c r="G187" s="28"/>
+      <c r="H187" s="28"/>
     </row>
     <row r="188" spans="7:8">
-      <c r="G188" s="30"/>
-      <c r="H188" s="30"/>
+      <c r="G188" s="28"/>
+      <c r="H188" s="28"/>
     </row>
     <row r="189" spans="7:8">
-      <c r="G189" s="30"/>
-      <c r="H189" s="30"/>
+      <c r="G189" s="28"/>
+      <c r="H189" s="28"/>
     </row>
     <row r="190" spans="7:8">
-      <c r="G190" s="30"/>
-      <c r="H190" s="30"/>
+      <c r="G190" s="28"/>
+      <c r="H190" s="28"/>
     </row>
     <row r="191" spans="7:8">
-      <c r="G191" s="30"/>
-      <c r="H191" s="30"/>
+      <c r="G191" s="28"/>
+      <c r="H191" s="28"/>
     </row>
     <row r="192" spans="7:8">
-      <c r="G192" s="30"/>
-      <c r="H192" s="30"/>
+      <c r="G192" s="28"/>
+      <c r="H192" s="28"/>
     </row>
     <row r="193" spans="7:8">
-      <c r="G193" s="30"/>
-      <c r="H193" s="30"/>
+      <c r="G193" s="28"/>
+      <c r="H193" s="28"/>
     </row>
     <row r="194" spans="7:8">
-      <c r="G194" s="30"/>
-      <c r="H194" s="30"/>
+      <c r="G194" s="28"/>
+      <c r="H194" s="28"/>
     </row>
     <row r="195" spans="7:8">
-      <c r="G195" s="30"/>
-      <c r="H195" s="30"/>
+      <c r="G195" s="28"/>
+      <c r="H195" s="28"/>
     </row>
     <row r="196" spans="7:8">
-      <c r="G196" s="30"/>
-      <c r="H196" s="30"/>
+      <c r="G196" s="28"/>
+      <c r="H196" s="28"/>
     </row>
     <row r="197" spans="7:8">
-      <c r="G197" s="30"/>
-      <c r="H197" s="30"/>
+      <c r="G197" s="28"/>
+      <c r="H197" s="28"/>
     </row>
     <row r="198" spans="7:8">
-      <c r="G198" s="30"/>
-      <c r="H198" s="30"/>
+      <c r="G198" s="28"/>
+      <c r="H198" s="28"/>
     </row>
     <row r="199" spans="7:8" ht="15.75" customHeight="1">
-      <c r="G199" s="30"/>
-      <c r="H199" s="30"/>
+      <c r="G199" s="28"/>
+      <c r="H199" s="28"/>
     </row>
     <row r="200" spans="7:8" ht="15.75" customHeight="1">
-      <c r="G200" s="30"/>
-      <c r="H200" s="30"/>
+      <c r="G200" s="28"/>
+      <c r="H200" s="28"/>
     </row>
     <row r="201" spans="7:8" ht="15.75" customHeight="1">
-      <c r="G201" s="30"/>
-      <c r="H201" s="30"/>
+      <c r="G201" s="28"/>
+      <c r="H201" s="28"/>
     </row>
     <row r="202" spans="7:8" ht="15.75" customHeight="1">
-      <c r="G202" s="30"/>
-      <c r="H202" s="30"/>
+      <c r="G202" s="28"/>
+      <c r="H202" s="28"/>
     </row>
     <row r="203" spans="7:8" ht="15.75" customHeight="1">
-      <c r="G203" s="30"/>
-      <c r="H203" s="30"/>
+      <c r="G203" s="28"/>
+      <c r="H203" s="28"/>
     </row>
     <row r="204" spans="7:8" ht="15.75" customHeight="1">
-      <c r="G204" s="30"/>
-      <c r="H204" s="30"/>
+      <c r="G204" s="28"/>
+      <c r="H204" s="28"/>
     </row>
     <row r="205" spans="7:8" ht="15.75" customHeight="1">
-      <c r="G205" s="30"/>
-      <c r="H205" s="30"/>
+      <c r="G205" s="28"/>
+      <c r="H205" s="28"/>
     </row>
     <row r="206" spans="7:8" ht="15.75" customHeight="1">
-      <c r="G206" s="30"/>
-      <c r="H206" s="30"/>
+      <c r="G206" s="28"/>
+      <c r="H206" s="28"/>
     </row>
     <row r="207" spans="7:8" ht="15.75" customHeight="1">
-      <c r="G207" s="30"/>
-      <c r="H207" s="30"/>
+      <c r="G207" s="28"/>
+      <c r="H207" s="28"/>
     </row>
     <row r="208" spans="7:8" ht="15.75" customHeight="1">
-      <c r="G208" s="30"/>
-      <c r="H208" s="30"/>
+      <c r="G208" s="28"/>
+      <c r="H208" s="28"/>
     </row>
     <row r="209" spans="7:8" ht="15.75" customHeight="1">
-      <c r="G209" s="30"/>
-      <c r="H209" s="30"/>
+      <c r="G209" s="28"/>
+      <c r="H209" s="28"/>
     </row>
     <row r="210" spans="7:8" ht="15.75" customHeight="1">
-      <c r="G210" s="30"/>
-      <c r="H210" s="30"/>
+      <c r="G210" s="28"/>
+      <c r="H210" s="28"/>
     </row>
     <row r="211" spans="7:8" ht="15.75" customHeight="1">
-      <c r="G211" s="30"/>
-      <c r="H211" s="30"/>
+      <c r="G211" s="28"/>
+      <c r="H211" s="28"/>
     </row>
     <row r="212" spans="7:8" ht="15.75" customHeight="1">
-      <c r="G212" s="30"/>
-      <c r="H212" s="30"/>
+      <c r="G212" s="28"/>
+      <c r="H212" s="28"/>
     </row>
     <row r="213" spans="7:8" ht="15.75" customHeight="1">
-      <c r="G213" s="30"/>
-      <c r="H213" s="30"/>
+      <c r="G213" s="28"/>
+      <c r="H213" s="28"/>
     </row>
     <row r="214" spans="7:8" ht="15.75" customHeight="1">
-      <c r="G214" s="30"/>
-      <c r="H214" s="30"/>
+      <c r="G214" s="28"/>
+      <c r="H214" s="28"/>
     </row>
     <row r="215" spans="7:8" ht="15.75" customHeight="1">
-      <c r="G215" s="30"/>
-      <c r="H215" s="30"/>
+      <c r="G215" s="28"/>
+      <c r="H215" s="28"/>
     </row>
     <row r="216" spans="7:8" ht="15.75" customHeight="1">
-      <c r="G216" s="30"/>
-      <c r="H216" s="30"/>
+      <c r="G216" s="28"/>
+      <c r="H216" s="28"/>
     </row>
     <row r="217" spans="7:8" ht="15.75" customHeight="1">
-      <c r="G217" s="30"/>
-      <c r="H217" s="30"/>
+      <c r="G217" s="28"/>
+      <c r="H217" s="28"/>
     </row>
     <row r="218" spans="7:8" ht="15.75" customHeight="1">
-      <c r="G218" s="30"/>
-      <c r="H218" s="30"/>
+      <c r="G218" s="28"/>
+      <c r="H218" s="28"/>
     </row>
     <row r="219" spans="7:8" ht="15.75" customHeight="1">
-      <c r="G219" s="30"/>
-      <c r="H219" s="30"/>
+      <c r="G219" s="28"/>
+      <c r="H219" s="28"/>
     </row>
     <row r="220" spans="7:8" ht="15.75" customHeight="1">
-      <c r="G220" s="30"/>
-      <c r="H220" s="30"/>
+      <c r="G220" s="28"/>
+      <c r="H220" s="28"/>
     </row>
     <row r="221" spans="7:8" ht="15.75" customHeight="1">
-      <c r="G221" s="30"/>
-      <c r="H221" s="30"/>
+      <c r="G221" s="28"/>
+      <c r="H221" s="28"/>
     </row>
     <row r="222" spans="7:8" ht="15.75" customHeight="1">
-      <c r="G222" s="30"/>
-      <c r="H222" s="30"/>
+      <c r="G222" s="28"/>
+      <c r="H222" s="28"/>
     </row>
     <row r="223" spans="7:8" ht="15.75" customHeight="1">
-      <c r="G223" s="30"/>
-      <c r="H223" s="30"/>
+      <c r="G223" s="28"/>
+      <c r="H223" s="28"/>
     </row>
     <row r="224" spans="7:8" ht="15.75" customHeight="1">
-      <c r="G224" s="28"/>
-      <c r="H224" s="28"/>
+      <c r="G224" s="26"/>
+      <c r="H224" s="26"/>
     </row>
     <row r="225" spans="7:8" ht="15.75" customHeight="1">
-      <c r="G225" s="28"/>
-      <c r="H225" s="28"/>
+      <c r="G225" s="26"/>
+      <c r="H225" s="26"/>
     </row>
     <row r="226" spans="7:8" ht="15.75" customHeight="1">
-      <c r="G226" s="28"/>
-      <c r="H226" s="28"/>
+      <c r="G226" s="26"/>
+      <c r="H226" s="26"/>
     </row>
     <row r="227" spans="7:8" ht="15.75" customHeight="1">
-      <c r="G227" s="28"/>
-      <c r="H227" s="28"/>
+      <c r="G227" s="26"/>
+      <c r="H227" s="26"/>
     </row>
     <row r="228" spans="7:8" ht="15.75" customHeight="1">
-      <c r="G228" s="28"/>
-      <c r="H228" s="28"/>
+      <c r="G228" s="26"/>
+      <c r="H228" s="26"/>
     </row>
     <row r="229" spans="7:8" ht="15.75" customHeight="1">
-      <c r="G229" s="28"/>
-      <c r="H229" s="28"/>
+      <c r="G229" s="26"/>
+      <c r="H229" s="26"/>
     </row>
     <row r="230" spans="7:8" ht="15.75" customHeight="1">
-      <c r="G230" s="28"/>
-      <c r="H230" s="28"/>
+      <c r="G230" s="26"/>
+      <c r="H230" s="26"/>
     </row>
     <row r="231" spans="7:8" ht="15.75" customHeight="1">
-      <c r="G231" s="28"/>
-      <c r="H231" s="28"/>
+      <c r="G231" s="26"/>
+      <c r="H231" s="26"/>
     </row>
     <row r="232" spans="7:8" ht="15.75" customHeight="1">
-      <c r="G232" s="28"/>
-      <c r="H232" s="28"/>
+      <c r="G232" s="26"/>
+      <c r="H232" s="26"/>
     </row>
     <row r="233" spans="7:8" ht="15.75" customHeight="1">
-      <c r="G233" s="28"/>
-      <c r="H233" s="28"/>
+      <c r="G233" s="26"/>
+      <c r="H233" s="26"/>
     </row>
     <row r="234" spans="7:8" ht="15.75" customHeight="1">
-      <c r="G234" s="28"/>
-      <c r="H234" s="28"/>
+      <c r="G234" s="26"/>
+      <c r="H234" s="26"/>
     </row>
     <row r="235" spans="7:8" ht="15.75" customHeight="1">
-      <c r="G235" s="28"/>
-      <c r="H235" s="28"/>
+      <c r="G235" s="26"/>
+      <c r="H235" s="26"/>
     </row>
     <row r="236" spans="7:8" ht="15.75" customHeight="1">
-      <c r="G236" s="28"/>
-      <c r="H236" s="28"/>
+      <c r="G236" s="26"/>
+      <c r="H236" s="26"/>
     </row>
     <row r="237" spans="7:8" ht="15.75" customHeight="1">
-      <c r="G237" s="28"/>
-      <c r="H237" s="28"/>
+      <c r="G237" s="26"/>
+      <c r="H237" s="26"/>
     </row>
     <row r="238" spans="7:8" ht="15.75" customHeight="1">
-      <c r="G238" s="28"/>
-      <c r="H238" s="28"/>
+      <c r="G238" s="26"/>
+      <c r="H238" s="26"/>
     </row>
     <row r="239" spans="7:8" ht="15.75" customHeight="1">
-      <c r="G239" s="28"/>
-      <c r="H239" s="28"/>
+      <c r="G239" s="26"/>
+      <c r="H239" s="26"/>
     </row>
     <row r="240" spans="7:8" ht="15.75" customHeight="1">
-      <c r="G240" s="28"/>
-      <c r="H240" s="28"/>
+      <c r="G240" s="26"/>
+      <c r="H240" s="26"/>
     </row>
     <row r="241" spans="7:8" ht="15.75" customHeight="1">
-      <c r="G241" s="28"/>
-      <c r="H241" s="28"/>
+      <c r="G241" s="26"/>
+      <c r="H241" s="26"/>
     </row>
     <row r="242" spans="7:8" ht="15.75" customHeight="1">
-      <c r="G242" s="28"/>
-      <c r="H242" s="28"/>
+      <c r="G242" s="26"/>
+      <c r="H242" s="26"/>
     </row>
     <row r="243" spans="7:8" ht="15.75" customHeight="1">
-      <c r="G243" s="28"/>
-      <c r="H243" s="28"/>
+      <c r="G243" s="26"/>
+      <c r="H243" s="26"/>
     </row>
     <row r="244" spans="7:8" ht="15.75" customHeight="1">
-      <c r="G244" s="28"/>
-      <c r="H244" s="28"/>
+      <c r="G244" s="26"/>
+      <c r="H244" s="26"/>
     </row>
     <row r="245" spans="7:8" ht="15.75" customHeight="1">
-      <c r="G245" s="28"/>
-      <c r="H245" s="28"/>
+      <c r="G245" s="26"/>
+      <c r="H245" s="26"/>
     </row>
     <row r="246" spans="7:8" ht="15.75" customHeight="1">
-      <c r="G246" s="28"/>
-      <c r="H246" s="28"/>
+      <c r="G246" s="26"/>
+      <c r="H246" s="26"/>
     </row>
     <row r="247" spans="7:8" ht="15.75" customHeight="1"/>
     <row r="248" spans="7:8" ht="15.75" customHeight="1"/>

</xml_diff>